<commit_message>
Actualización escaleta CN 06 05
Actualización escaleta CN 06 05
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion05/Escaleta_CN_06_05_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion05/Escaleta_CN_06_05_CO.xlsx
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Escaleta!$A$2:$U$36</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1084,34 +1084,17 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1153,7 +1136,24 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1491,94 +1491,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="15" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="32" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="P1" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="38" t="s">
+      <c r="R1" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="U1" s="50" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="47"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="16" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="35"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="51"/>
     </row>
     <row r="3" spans="1:21" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1611,7 +1611,7 @@
         <v>20</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>57</v>
@@ -2253,7 +2253,7 @@
         <v>32</v>
       </c>
       <c r="O14" s="21"/>
-      <c r="P14" s="55" t="s">
+      <c r="P14" s="32" t="s">
         <v>20</v>
       </c>
       <c r="Q14" s="10">
@@ -2423,7 +2423,7 @@
         <v>19</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="M17" s="8" t="s">
         <v>62</v>
@@ -2668,7 +2668,7 @@
         <v>32</v>
       </c>
       <c r="O21" s="21"/>
-      <c r="P21" s="55" t="s">
+      <c r="P21" s="32" t="s">
         <v>20</v>
       </c>
       <c r="Q21" s="10">
@@ -3076,7 +3076,7 @@
         <v>32</v>
       </c>
       <c r="O29" s="21"/>
-      <c r="P29" s="55" t="s">
+      <c r="P29" s="32" t="s">
         <v>20</v>
       </c>
       <c r="Q29" s="10">
@@ -3465,7 +3465,7 @@
         <v>52</v>
       </c>
       <c r="O36" s="21"/>
-      <c r="P36" s="55" t="s">
+      <c r="P36" s="32" t="s">
         <v>20</v>
       </c>
       <c r="Q36" s="10">
@@ -4584,6 +4584,12 @@
   </sheetData>
   <autoFilter ref="A2:U36"/>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4598,12 +4604,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización CN 06 05 (guion y escaleta)
Actualización CN 06 05 (guion y escaleta)
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion05/Escaleta_CN_06_05_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion05/Escaleta_CN_06_05_CO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="262">
   <si>
     <t>Asignatura</t>
   </si>
@@ -471,9 +471,6 @@
     <t>La pirámide alimentaria</t>
   </si>
   <si>
-    <t>Actividad que identifica las raciones diarias de alimentos que recomienda tomar la pirámide alimentaria</t>
-  </si>
-  <si>
     <t>Cambiar el título “Responde sobre alimentos y la pirámide alimentaria” por “La pirámide alimentaria”.</t>
   </si>
   <si>
@@ -564,9 +561,6 @@
     <t>RF_01_01_CO</t>
   </si>
   <si>
-    <t>Enfermedades asociadas al sistema digestivo</t>
-  </si>
-  <si>
     <t>Recurso M101A-04</t>
   </si>
   <si>
@@ -579,9 +573,6 @@
     <t>Competencias: comprensión de los nutrientes y sus características</t>
   </si>
   <si>
-    <t>Actividad que propone realizar la explicación de la acción de los nutrientes, su importancia en el organismo y como deben ser ingeridos</t>
-  </si>
-  <si>
     <t>Competencias: interpretación de las etiquetas de los alimentos</t>
   </si>
   <si>
@@ -636,9 +627,6 @@
     <t>Secuencia de imágenes que presenta los alimentos pertenecientes a los siete grandes grupos</t>
   </si>
   <si>
-    <t>Actividad para completar un texto que permita comprender el concepto de dieta equilibrada</t>
-  </si>
-  <si>
     <t>http://aulaplaneta.planetasaber.com/encyclopedia/asp/Preview15.asp?IdPack=15&amp;IdPildora=554848</t>
   </si>
   <si>
@@ -708,9 +696,6 @@
     <t>Los tipos de nutrientes en los alimentos</t>
   </si>
   <si>
-    <t>Los alimentos según los nutrientes que contienen</t>
-  </si>
-  <si>
     <t>Clasifica los alimentos según su función</t>
   </si>
   <si>
@@ -720,9 +705,6 @@
     <t>Actividad interactiva para clasificar los alimentos de acuerdo al tipo de nutrientes que presentan</t>
   </si>
   <si>
-    <t>¿Qué es la dieta equilibrada?</t>
-  </si>
-  <si>
     <t>La dieta equilibrada</t>
   </si>
   <si>
@@ -814,6 +796,21 @@
   </si>
   <si>
     <t>Banco de actividades del tema La nutrición y digestión en el ser humano</t>
+  </si>
+  <si>
+    <t>Actividad que identifica las raciones diarias de alimentos que se recomienda tomar según la pirámide alimentaria</t>
+  </si>
+  <si>
+    <t>¿Qué es una dieta equilibrada?</t>
+  </si>
+  <si>
+    <t>Las enfermedades asociadas al sistema digestivo</t>
+  </si>
+  <si>
+    <t>Actividad para completar un texto que permite comprender el concepto de dieta equilibrada</t>
+  </si>
+  <si>
+    <t>Actividad que permite la comprensión de la acción de los nutrientes, su importancia en el organismo y cómo deben ser ingeridos</t>
   </si>
 </sst>
 </file>
@@ -1461,9 +1458,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U282"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,7 +1585,7 @@
         <v>122</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>123</v>
@@ -1596,7 +1593,7 @@
       <c r="E3" s="12"/>
       <c r="F3" s="9"/>
       <c r="G3" s="17" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="H3" s="9">
         <v>1</v>
@@ -1605,7 +1602,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1625,16 +1622,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="S3" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="T3" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="U3" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="T3" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1645,7 +1642,7 @@
         <v>122</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>123</v>
@@ -1655,7 +1652,7 @@
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="17" t="s">
-        <v>227</v>
+        <v>126</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
@@ -1664,7 +1661,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>19</v>
@@ -1704,7 +1701,7 @@
         <v>122</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>123</v>
@@ -1714,7 +1711,7 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="17" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
@@ -1723,7 +1720,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1763,7 +1760,7 @@
         <v>122</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>123</v>
@@ -1798,7 +1795,7 @@
         <v>122</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>123</v>
@@ -1810,7 +1807,7 @@
         <v>131</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H7" s="9">
         <v>4</v>
@@ -1819,7 +1816,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -1859,7 +1856,7 @@
         <v>122</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>123</v>
@@ -1871,7 +1868,7 @@
         <v>133</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H8" s="9">
         <v>5</v>
@@ -1880,7 +1877,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -1920,7 +1917,7 @@
         <v>122</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>123</v>
@@ -1932,7 +1929,7 @@
         <v>133</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H9" s="9">
         <v>6</v>
@@ -1941,7 +1938,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>20</v>
@@ -1967,7 +1964,7 @@
         <v>127</v>
       </c>
       <c r="T9" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U9" s="10" t="s">
         <v>129</v>
@@ -1981,7 +1978,7 @@
         <v>122</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>123</v>
@@ -2000,7 +1997,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -2040,13 +2037,13 @@
         <v>122</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>147</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="17" t="s">
@@ -2072,7 +2069,7 @@
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="21" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="P11" s="9" t="s">
         <v>19</v>
@@ -2101,13 +2098,13 @@
         <v>122</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>147</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="17" t="s">
@@ -2120,7 +2117,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>148</v>
+        <v>257</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>19</v>
@@ -2133,7 +2130,7 @@
         <v>33</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>19</v>
@@ -2148,7 +2145,7 @@
         <v>145</v>
       </c>
       <c r="T12" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U12" s="10" t="s">
         <v>146</v>
@@ -2162,17 +2159,17 @@
         <v>122</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>147</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="17" t="s">
-        <v>231</v>
+        <v>258</v>
       </c>
       <c r="H13" s="9">
         <v>10</v>
@@ -2181,7 +2178,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>203</v>
+        <v>260</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2207,7 +2204,7 @@
         <v>127</v>
       </c>
       <c r="T13" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="U13" s="10" t="s">
         <v>129</v>
@@ -2221,17 +2218,17 @@
         <v>122</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>147</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="H14" s="9">
         <v>11</v>
@@ -2240,7 +2237,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -2280,7 +2277,7 @@
         <v>122</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>147</v>
@@ -2290,7 +2287,7 @@
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H15" s="9">
         <v>12</v>
@@ -2299,7 +2296,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>19</v>
@@ -2325,7 +2322,7 @@
         <v>145</v>
       </c>
       <c r="T15" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="U15" s="10" t="s">
         <v>146</v>
@@ -2339,17 +2336,17 @@
         <v>122</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H16" s="9">
         <v>13</v>
@@ -2358,7 +2355,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>19</v>
@@ -2384,7 +2381,7 @@
         <v>145</v>
       </c>
       <c r="T16" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U16" s="10" t="s">
         <v>146</v>
@@ -2398,17 +2395,17 @@
         <v>122</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H17" s="9">
         <v>14</v>
@@ -2417,7 +2414,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>19</v>
@@ -2443,7 +2440,7 @@
         <v>145</v>
       </c>
       <c r="T17" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="U17" s="10" t="s">
         <v>146</v>
@@ -2457,17 +2454,17 @@
         <v>122</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="17" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="H18" s="9">
         <v>15</v>
@@ -2476,7 +2473,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2496,13 +2493,13 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S18" s="19" t="s">
         <v>127</v>
       </c>
       <c r="T18" s="20" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="U18" s="10" t="s">
         <v>129</v>
@@ -2516,17 +2513,17 @@
         <v>122</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H19" s="9">
         <v>16</v>
@@ -2535,7 +2532,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>19</v>
@@ -2548,7 +2545,7 @@
         <v>28</v>
       </c>
       <c r="O19" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>19</v>
@@ -2563,7 +2560,7 @@
         <v>145</v>
       </c>
       <c r="T19" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U19" s="10" t="s">
         <v>146</v>
@@ -2577,17 +2574,17 @@
         <v>122</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H20" s="9">
         <v>17</v>
@@ -2596,7 +2593,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2622,7 +2619,7 @@
         <v>127</v>
       </c>
       <c r="T20" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U20" s="10" t="s">
         <v>129</v>
@@ -2636,17 +2633,17 @@
         <v>122</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="17" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="H21" s="9">
         <v>18</v>
@@ -2655,7 +2652,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2681,7 +2678,7 @@
         <v>127</v>
       </c>
       <c r="T21" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U21" s="10" t="s">
         <v>129</v>
@@ -2695,17 +2692,17 @@
         <v>122</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>135</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="17" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H22" s="9">
         <v>19</v>
@@ -2714,7 +2711,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2740,7 +2737,7 @@
         <v>127</v>
       </c>
       <c r="T22" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U22" s="10" t="s">
         <v>129</v>
@@ -2754,16 +2751,16 @@
         <v>122</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="9"/>
@@ -2789,16 +2786,16 @@
         <v>122</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="9"/>
@@ -2824,16 +2821,16 @@
         <v>122</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="9"/>
@@ -2859,19 +2856,19 @@
         <v>122</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>179</v>
+        <v>259</v>
       </c>
       <c r="H26" s="9">
         <v>20</v>
@@ -2880,7 +2877,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>
@@ -2906,7 +2903,7 @@
         <v>127</v>
       </c>
       <c r="T26" s="20" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="U26" s="10" t="s">
         <v>129</v>
@@ -2920,19 +2917,19 @@
         <v>122</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H27" s="9">
         <v>21</v>
@@ -2941,7 +2938,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>20</v>
@@ -2967,7 +2964,7 @@
         <v>127</v>
       </c>
       <c r="T27" s="20" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="U27" s="10" t="s">
         <v>129</v>
@@ -2981,19 +2978,19 @@
         <v>122</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H28" s="9">
         <v>22</v>
@@ -3002,7 +2999,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>20</v>
@@ -3011,7 +3008,7 @@
         <v>5</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="N28" s="8"/>
       <c r="O28" s="21"/>
@@ -3022,16 +3019,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="S28" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="S28" s="19" t="s">
+      <c r="T28" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="U28" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="T28" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="U28" s="10" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3042,19 +3039,19 @@
         <v>122</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="H29" s="9">
         <v>23</v>
@@ -3063,7 +3060,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>20</v>
@@ -3089,7 +3086,7 @@
         <v>127</v>
       </c>
       <c r="T29" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U29" s="10" t="s">
         <v>129</v>
@@ -3103,17 +3100,17 @@
         <v>122</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>135</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="17" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="H30" s="9">
         <v>24</v>
@@ -3122,7 +3119,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="18" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>20</v>
@@ -3148,13 +3145,13 @@
         <v>127</v>
       </c>
       <c r="T30" s="20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="U30" s="10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>17</v>
       </c>
@@ -3162,15 +3159,15 @@
         <v>122</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="9"/>
       <c r="G31" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H31" s="9">
         <v>25</v>
@@ -3179,7 +3176,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>184</v>
+        <v>261</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>19</v>
@@ -3205,7 +3202,7 @@
         <v>145</v>
       </c>
       <c r="T31" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="U31" s="10" t="s">
         <v>146</v>
@@ -3219,15 +3216,15 @@
         <v>122</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="9"/>
       <c r="G32" s="17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H32" s="9">
         <v>26</v>
@@ -3236,7 +3233,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="18" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>19</v>
@@ -3262,7 +3259,7 @@
         <v>145</v>
       </c>
       <c r="T32" s="20" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="U32" s="10" t="s">
         <v>146</v>
@@ -3276,15 +3273,15 @@
         <v>122</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="9"/>
       <c r="G33" s="17" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H33" s="9">
         <v>27</v>
@@ -3293,7 +3290,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="18" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>19</v>
@@ -3319,7 +3316,7 @@
         <v>145</v>
       </c>
       <c r="T33" s="20" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="U33" s="10" t="s">
         <v>146</v>
@@ -3333,15 +3330,15 @@
         <v>122</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="9"/>
       <c r="G34" s="17" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H34" s="9">
         <v>28</v>
@@ -3350,7 +3347,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3378,15 +3375,15 @@
         <v>122</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="9"/>
       <c r="G35" s="17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H35" s="9">
         <v>29</v>
@@ -3395,7 +3392,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="18" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
@@ -3421,7 +3418,7 @@
         <v>127</v>
       </c>
       <c r="T35" s="20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="U35" s="10" t="s">
         <v>129</v>
@@ -3435,15 +3432,15 @@
         <v>122</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="9"/>
       <c r="G36" s="17" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H36" s="9">
         <v>30</v>
@@ -3452,7 +3449,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="K36" s="7" t="s">
         <v>20</v>
@@ -3478,7 +3475,7 @@
         <v>127</v>
       </c>
       <c r="T36" s="20" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="U36" s="10" t="s">
         <v>129</v>
@@ -4666,19 +4663,19 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="E2" s="23" t="s">
         <v>197</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4690,10 +4687,10 @@
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="27" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4705,109 +4702,109 @@
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="27" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>154</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>155</v>
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="27" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>154</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>155</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="27" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
       <c r="D7" s="27" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="26"/>
       <c r="D8" s="27" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="C9" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>173</v>
-      </c>
       <c r="D9" s="27" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="30" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E12" s="31"/>
     </row>

</xml_diff>